<commit_message>
working login, acceptance plan updated
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>User Story</t>
   </si>
@@ -651,7 +651,7 @@
     <col min="6" max="6" style="8" width="60.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -671,7 +671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60" customFormat="1" s="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -701,14 +701,16 @@
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60" customFormat="1" s="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
@@ -720,14 +722,16 @@
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="46.5" customFormat="1" s="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
@@ -748,7 +752,9 @@
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
@@ -760,7 +766,9 @@
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
@@ -802,7 +810,9 @@
       <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
@@ -814,7 +824,9 @@
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>31</v>
       </c>

</xml_diff>